<commit_message>
change msword lib from win32com to python-docx
</commit_message>
<xml_diff>
--- a/resource/test.xlsx
+++ b/resource/test.xlsx
@@ -7,23 +7,23 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="18180" windowHeight="8325"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="titles" sheetId="2" r:id="rId1"/>
+    <sheet name="vuls" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc421788828" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="_Toc421788829" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="_Toc421788830" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="_Toc421788831" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="_Toc421788832" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="_Toc421788828" localSheetId="1">vuls!#REF!</definedName>
+    <definedName name="_Toc421788829" localSheetId="1">vuls!#REF!</definedName>
+    <definedName name="_Toc421788830" localSheetId="1">vuls!#REF!</definedName>
+    <definedName name="_Toc421788831" localSheetId="1">vuls!#REF!</definedName>
+    <definedName name="_Toc421788832" localSheetId="1">vuls!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>website</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,46 @@
   </si>
   <si>
     <t>這裡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title1.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title3.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title3.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,9 +482,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -532,19 +660,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>

</xml_diff>